<commit_message>
HSV Simples e HSV Multipatamar ok
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Python Scripts\Calculadora-de-Demanda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23907BD-B1BA-4CE9-855F-372CE6AD7756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271F9DA8-0E55-439C-B0DA-D4B126FF2134}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,9 +139,9 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,8 +177,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <u val="singleAccounting"/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,6 +195,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -283,7 +296,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -292,12 +305,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -313,10 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -330,9 +334,6 @@
     <xf numFmtId="17" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -342,9 +343,29 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -664,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,12 +703,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="4"/>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,454 +735,454 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="23">
         <v>65</v>
       </c>
-      <c r="G2" s="10">
-        <v>0</v>
-      </c>
-      <c r="H2" s="10">
+      <c r="G2" s="8">
+        <v>0</v>
+      </c>
+      <c r="H2" s="21">
         <v>58.8</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="21">
         <v>63.39</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="22">
         <v>5330</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="22">
         <v>977</v>
       </c>
-      <c r="L2" s="12">
+      <c r="L2" s="9">
         <v>0.15490724591723481</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="11">
         <v>1.25116</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="26">
         <v>1.9790572603606453</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="23">
         <v>65</v>
       </c>
-      <c r="G3" s="10">
-        <v>0</v>
-      </c>
-      <c r="H3" s="10">
+      <c r="G3" s="8">
+        <v>0</v>
+      </c>
+      <c r="H3" s="21">
         <v>58.91</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="21">
         <v>52.19</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="22">
         <v>5429</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="22">
         <v>945</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="9">
         <v>0.14825855036084093</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="11">
         <v>0.33783999999999997</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="25">
         <v>0.5343878519455868</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="23">
         <v>95</v>
       </c>
-      <c r="G4" s="10">
-        <v>0</v>
-      </c>
-      <c r="H4" s="10">
+      <c r="G4" s="8">
+        <v>0</v>
+      </c>
+      <c r="H4" s="21">
         <v>46.48</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="21">
         <v>20.16</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="22">
         <v>7837</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="22">
         <v>1196</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="9">
         <v>0.13240340971991588</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="11">
         <v>20.38</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="25">
         <v>32.236633976589687</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="23">
         <v>95</v>
       </c>
-      <c r="G5" s="10">
-        <v>0</v>
-      </c>
-      <c r="H5" s="10">
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5" s="21">
         <v>63.17</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="21">
         <v>39.979999999999997</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="22">
         <v>6251</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="22">
         <v>932</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="9">
         <v>0.12975080050118334</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="11">
         <v>40.76</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="25">
         <v>64.473267953179374</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="23">
         <v>95</v>
       </c>
-      <c r="G6" s="10">
-        <v>0</v>
-      </c>
-      <c r="H6" s="10">
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="21">
         <v>59.47</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="21">
         <v>47.71</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="22">
         <v>7162</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="22">
         <v>1217</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="9">
         <v>0.14524406253729563</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="9" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="23">
         <v>95</v>
       </c>
-      <c r="G7" s="10">
-        <v>0</v>
-      </c>
-      <c r="H7" s="10">
+      <c r="G7" s="8">
+        <v>0</v>
+      </c>
+      <c r="H7" s="21">
         <v>61.04</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="21">
         <v>46.37</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="22">
         <v>8539</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="22">
         <v>1304</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="9">
         <v>0.13247993497917301</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="23">
         <v>95</v>
       </c>
-      <c r="G8" s="10">
-        <v>0</v>
-      </c>
-      <c r="H8" s="10">
+      <c r="G8" s="8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="21">
         <v>81.98</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="21">
         <v>53.09</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="22">
         <v>10174</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="22">
         <v>1741</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="9">
         <v>0.14611833822912296</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="11">
         <v>0.50831000000000004</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="11">
         <v>0.8040335336918697</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="23">
         <v>95</v>
       </c>
-      <c r="G9" s="10">
-        <v>0</v>
-      </c>
-      <c r="H9" s="10">
+      <c r="G9" s="8">
+        <v>0</v>
+      </c>
+      <c r="H9" s="21">
         <v>77.62</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="21">
         <v>77.73</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="22">
         <v>11921</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="22">
         <v>2337</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="9">
         <v>0.16390798148407912</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="11">
         <v>0.33783999999999997</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="11">
         <v>0.5343878519455868</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="23">
         <v>95</v>
       </c>
-      <c r="G10" s="10">
-        <v>0</v>
-      </c>
-      <c r="H10" s="10">
+      <c r="G10" s="8">
+        <v>0</v>
+      </c>
+      <c r="H10" s="21">
         <v>89.49</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="21">
         <v>61.82</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="22">
         <v>15381</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="22">
         <v>2781</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="9">
         <v>0.1531219028741328</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="11">
         <v>30.45</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="11">
         <v>48.165137614678898</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="23">
         <v>95</v>
       </c>
-      <c r="G11" s="10">
-        <v>0</v>
-      </c>
-      <c r="H11" s="10">
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+      <c r="H11" s="21">
         <v>81.09</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="21">
         <v>57.12</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="22">
         <v>12332</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="22">
         <v>2140</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="9">
         <v>0.14787175234936428</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="11">
         <v>20.38</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="11">
         <v>32.236633976589687</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="23">
         <v>95</v>
       </c>
-      <c r="G12" s="10">
-        <v>0</v>
-      </c>
-      <c r="H12" s="10">
+      <c r="G12" s="8">
+        <v>0</v>
+      </c>
+      <c r="H12" s="21">
         <v>66.98</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="21">
         <v>56.9</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="22">
         <v>12623</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="22">
         <v>2084</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="9">
         <v>0.14170123070646631</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="11">
         <v>60.9</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="11">
         <v>96.330275229357795</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="23">
         <v>75</v>
       </c>
-      <c r="G13" s="10">
-        <v>0</v>
-      </c>
-      <c r="H13" s="10">
-        <v>66.42</v>
-      </c>
-      <c r="I13" s="10">
+      <c r="G13" s="8">
+        <v>0</v>
+      </c>
+      <c r="H13" s="21">
+        <v>85</v>
+      </c>
+      <c r="I13" s="21">
         <v>40.659999999999997</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="22">
         <v>7074</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="22">
         <v>1353</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="9">
         <v>0.16055535777856889</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="11">
         <v>40.76</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="11">
         <v>64.473267953179374</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="24">
         <v>88.333333333333329</v>
       </c>
-      <c r="G14" s="19">
-        <v>0</v>
-      </c>
-      <c r="H14" s="20">
+      <c r="G14" s="15">
+        <v>0</v>
+      </c>
+      <c r="H14" s="16">
         <v>67.620833333333337</v>
       </c>
-      <c r="I14" s="20">
+      <c r="I14" s="16">
         <v>51.426666666666655</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="17">
         <v>9171.0833333333339</v>
       </c>
-      <c r="K14" s="21">
+      <c r="K14" s="17">
         <v>1583.9166666666667</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="18">
         <v>0.14636004728644814</v>
       </c>
     </row>
@@ -1171,5 +1192,6 @@
     <mergeCell ref="A7:C7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>